<commit_message>
added a realtime test data for the project
</commit_message>
<xml_diff>
--- a/data/requirements.xlsx
+++ b/data/requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanb/BPAOT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AFED55-04B4-1344-9F38-34DFF31D193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AAAD20-24CC-BD46-B48E-E00DBB2C5DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Requirement</t>
   </si>
@@ -31,22 +31,76 @@
     <t>Proposed Solution</t>
   </si>
   <si>
-    <t>Track leave request status</t>
-  </si>
-  <si>
-    <t>Employees are unsure of their request’s progress</t>
-  </si>
-  <si>
-    <t>Add a real-time status tracker</t>
-  </si>
-  <si>
-    <t>Digitize approval process</t>
-  </si>
-  <si>
-    <t>Managers approve via email, which is hard to track</t>
-  </si>
-  <si>
-    <t>Build a centralized approval dashboard</t>
+    <t>Track leave requests</t>
+  </si>
+  <si>
+    <t>Employees don’t know request status</t>
+  </si>
+  <si>
+    <t>Add real-time tracking in the HR portal</t>
+  </si>
+  <si>
+    <t>Centralize approvals</t>
+  </si>
+  <si>
+    <t>Managers respond via scattered emails</t>
+  </si>
+  <si>
+    <t>Create a centralized approval dashboard</t>
+  </si>
+  <si>
+    <t>Automate report generation</t>
+  </si>
+  <si>
+    <t>Manual monthly reporting is slow</t>
+  </si>
+  <si>
+    <t>Auto-generate PDF reports from database</t>
+  </si>
+  <si>
+    <t>Improve data search</t>
+  </si>
+  <si>
+    <t>Filtering records is time-consuming</t>
+  </si>
+  <si>
+    <t>Add a search and filter panel for users</t>
+  </si>
+  <si>
+    <t>Analyze process delays</t>
+  </si>
+  <si>
+    <t>No visibility into bottlenecks</t>
+  </si>
+  <si>
+    <t>Include timestamp logging and delay metrics</t>
+  </si>
+  <si>
+    <t>Summarize user feedback</t>
+  </si>
+  <si>
+    <t>Unstructured notes are hard to review</t>
+  </si>
+  <si>
+    <t>Store feedback with sentiment tagging</t>
+  </si>
+  <si>
+    <t>Visualize data trends</t>
+  </si>
+  <si>
+    <t>Stakeholders don’t understand raw data</t>
+  </si>
+  <si>
+    <t>Use bar charts and KPIs in reports</t>
+  </si>
+  <si>
+    <t>Reduce duplicate requests</t>
+  </si>
+  <si>
+    <t>Employees submit same requests twice</t>
+  </si>
+  <si>
+    <t>Add validation for existing entries</t>
   </si>
 </sst>
 </file>
@@ -65,6 +119,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,14 +464,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="51.5" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -452,6 +510,72 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>